<commit_message>
Changed graph axis defaults to better reflect dispayed data
</commit_message>
<xml_diff>
--- a/RequestedOps vs. Achieved at Latency.xlsx
+++ b/RequestedOps vs. Achieved at Latency.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Isilon\Work\Samsung CAE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Isilon\GitHub\excel_ops_vs_latency_and_ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -414,49 +414,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
                 <c:pt idx="0">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>#N/A</c:v>
@@ -876,8 +876,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199422568"/>
-        <c:axId val="199422176"/>
+        <c:axId val="189972840"/>
+        <c:axId val="189973232"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1057,49 +1057,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
                 <c:pt idx="0">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>236363</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>#N/A</c:v>
@@ -1519,11 +1519,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198234336"/>
-        <c:axId val="198230808"/>
+        <c:axId val="189974016"/>
+        <c:axId val="189973624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="199422568"/>
+        <c:axId val="189972840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200000"/>
@@ -1553,14 +1553,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199422176"/>
+        <c:crossAx val="189973232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199422176"/>
+        <c:axId val="189973232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1588,14 +1590,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199422568"/>
+        <c:crossAx val="189972840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198230808"/>
+        <c:axId val="189973624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="300000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1622,12 +1627,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198234336"/>
+        <c:crossAx val="189974016"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198234336"/>
+        <c:axId val="189974016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198230808"/>
+        <c:crossAx val="189973624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1664,7 +1669,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Helpers!$I$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Helpers!$I$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2174,7 +2179,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="10">
-        <v>2.7</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -2764,11 +2769,11 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>IF(OR(ISBLANK('Latency Data'!B2), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B2),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2776,17 +2781,17 @@
         <v>1</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>IF(OR(ISBLANK('Latency Data'!B3), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B3),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2794,11 +2799,11 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>IF(OR(ISBLANK('Latency Data'!B4), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B4),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2806,11 +2811,11 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>IF(OR(ISBLANK('Latency Data'!B5), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B5),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -2818,11 +2823,11 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>IF(OR(ISBLANK('Latency Data'!B6), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B6),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2830,11 +2835,11 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>IF(OR(ISBLANK('Latency Data'!B7), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B7),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2842,11 +2847,11 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>IF(OR(ISBLANK('Latency Data'!B8), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B8),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2854,11 +2859,11 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>IF(OR(ISBLANK('Latency Data'!B9), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B9),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2866,11 +2871,11 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>IF(OR(ISBLANK('Latency Data'!B10), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!B10),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2878,11 +2883,11 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2890,11 +2895,11 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2902,11 +2907,11 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2914,11 +2919,11 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2926,11 +2931,11 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2938,11 +2943,11 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!), NOT($H$2)),NA(),'Latency and Ops Graph'!$D$2)</f>
-        <v>2.7</v>
-      </c>
-      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="B16" t="e">
         <f>IF(OR(ISBLANK('Latency Data'!#REF!),NOT($I$2)),NA(),'Latency and Ops Graph'!$D$3)</f>
-        <v>236363</v>
+        <v>#N/A</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
Fix cell formatting on the latency data sheet
</commit_message>
<xml_diff>
--- a/RequestedOps vs. Achieved at Latency.xlsx
+++ b/RequestedOps vs. Achieved at Latency.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Syncplicity\Nitro-Alpha (William Griffith)\05-Results\KR-Samsung CAE (Beta)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Isilon\GitHub\excel_ops_vs_latency_and_ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -144,7 +144,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#.0#\ &quot;ms&quot;"/>
+    <numFmt numFmtId="167" formatCode="#.00\ &quot;ms&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -197,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -220,49 +220,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -273,7 +230,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -283,31 +240,22 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2352,8 +2300,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="418401960"/>
-        <c:axId val="339957312"/>
+        <c:axId val="253748624"/>
+        <c:axId val="330259696"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4300,11 +4248,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="339955744"/>
-        <c:axId val="339956920"/>
+        <c:axId val="339620552"/>
+        <c:axId val="339620160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="418401960"/>
+        <c:axId val="253748624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="410000"/>
@@ -4335,12 +4283,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339957312"/>
+        <c:crossAx val="330259696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339957312"/>
+        <c:axId val="330259696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -4372,13 +4320,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="418401960"/>
+        <c:crossAx val="253748624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339956920"/>
+        <c:axId val="339620160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350000"/>
@@ -4409,13 +4357,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339955744"/>
+        <c:crossAx val="339620552"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339955744"/>
+        <c:axId val="339620552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4425,7 +4373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339956920"/>
+        <c:crossAx val="339620160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5274,19 +5222,19 @@
       <c r="B2" s="2">
         <v>5000</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="15">
         <v>3280</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="11">
         <v>2.0699999999999998</v>
       </c>
       <c r="G2" s="2">
         <v>100000</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="14">
         <v>60066.400000000001</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="10">
         <v>1.3760407714843801</v>
       </c>
     </row>
@@ -5295,17 +5243,17 @@
         <f>B2+5000</f>
         <v>10000</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="15">
         <v>6280</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <v>2.2999999999999998</v>
       </c>
       <c r="G3" s="2">
         <f>G2+10000</f>
         <v>110000</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="14">
         <v>64288.200000000004</v>
       </c>
       <c r="I3" s="10">
@@ -5317,17 +5265,17 @@
         <f t="shared" ref="B4:B31" si="0">B3+5000</f>
         <v>15000</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="15">
         <v>9100</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <v>2.56</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G31" si="1">G3+10000</f>
         <v>120000</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="14">
         <v>68863.399999999994</v>
       </c>
       <c r="I4" s="10">
@@ -5339,17 +5287,17 @@
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="15">
         <v>12100</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <v>2.68</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="1"/>
         <v>130000</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="14">
         <v>73638.3</v>
       </c>
       <c r="I5" s="10">
@@ -5361,17 +5309,17 @@
         <f t="shared" si="0"/>
         <v>25000</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="15">
         <v>14900</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="11">
         <v>2.93</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="1"/>
         <v>140000</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="14">
         <v>78751.100000000006</v>
       </c>
       <c r="I6" s="10">
@@ -5383,17 +5331,17 @@
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="15">
         <v>17700</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="11">
         <v>3.07</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="1"/>
         <v>150000</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="14">
         <v>83877.2</v>
       </c>
       <c r="I7" s="10">
@@ -5405,17 +5353,17 @@
         <f t="shared" si="0"/>
         <v>35000</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="15">
         <v>20400</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <v>3.08</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="1"/>
         <v>160000</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="14">
         <v>89093</v>
       </c>
       <c r="I8" s="10">
@@ -5427,17 +5375,17 @@
         <f t="shared" si="0"/>
         <v>40000</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="15">
         <v>23600</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="11">
         <v>3.5</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="1"/>
         <v>170000</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="14">
         <v>94459.4</v>
       </c>
       <c r="I9" s="10">
@@ -5449,17 +5397,17 @@
         <f t="shared" si="0"/>
         <v>45000</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="15">
         <v>26400</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="11">
         <v>3.72</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="1"/>
         <v>180000</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="14">
         <v>99667.5</v>
       </c>
       <c r="I10" s="10">
@@ -5471,17 +5419,17 @@
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="15">
         <v>29000</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="11">
         <v>3.99</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="1"/>
         <v>190000</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="14">
         <v>104674</v>
       </c>
       <c r="I11" s="10">
@@ -5493,17 +5441,17 @@
         <f t="shared" si="0"/>
         <v>55000</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="15">
         <v>31500</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <v>4.0999999999999996</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="1"/>
         <v>200000</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="14">
         <v>109987</v>
       </c>
       <c r="I12" s="10">
@@ -5515,17 +5463,17 @@
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="15">
         <v>34200</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <v>4.3</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
         <v>210000</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="14">
         <v>115409</v>
       </c>
       <c r="I13" s="10">
@@ -5537,17 +5485,17 @@
         <f t="shared" si="0"/>
         <v>65000</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="15">
         <v>37600</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="11">
         <v>4.58</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
         <v>220000</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="14">
         <v>121102</v>
       </c>
       <c r="I14" s="10">
@@ -5559,17 +5507,17 @@
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="15">
         <v>40100</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="11">
         <v>4.74</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
         <v>230000</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="14">
         <v>126114</v>
       </c>
       <c r="I15" s="10">
@@ -5581,17 +5529,17 @@
         <f t="shared" si="0"/>
         <v>75000</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="15">
         <v>42600</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="11">
         <v>5.52</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
         <v>240000</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="14">
         <v>132452</v>
       </c>
       <c r="I16" s="10">
@@ -5603,17 +5551,17 @@
         <f t="shared" si="0"/>
         <v>80000</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="15">
         <v>45300</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="11">
         <v>6.1</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="1"/>
         <v>250000</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="14">
         <v>136067</v>
       </c>
       <c r="I17" s="10">
@@ -5625,17 +5573,17 @@
         <f t="shared" si="0"/>
         <v>85000</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="15">
         <v>48000</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="11">
         <v>6.81</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="1"/>
         <v>260000</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="14">
         <v>141665</v>
       </c>
       <c r="I18" s="10">
@@ -5647,17 +5595,17 @@
         <f t="shared" si="0"/>
         <v>90000</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="15">
         <v>50700</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="11">
         <v>8.5</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="1"/>
         <v>270000</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="14">
         <v>146926</v>
       </c>
       <c r="I19" s="10">
@@ -5669,17 +5617,17 @@
         <f t="shared" si="0"/>
         <v>95000</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="15">
         <v>53400</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="11">
         <v>11</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="1"/>
         <v>280000</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="14">
         <v>152292</v>
       </c>
       <c r="I20" s="10">
@@ -5691,17 +5639,17 @@
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="15">
         <v>56100</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="11">
         <v>14.3</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
         <v>290000</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="14">
         <v>157466</v>
       </c>
       <c r="I21" s="10">
@@ -5713,17 +5661,17 @@
         <f t="shared" si="0"/>
         <v>105000</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="15">
         <v>56200</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="11">
         <v>14.2</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="1"/>
         <v>300000</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="14">
         <v>163169</v>
       </c>
       <c r="I22" s="10">
@@ -5735,17 +5683,17 @@
         <f t="shared" si="0"/>
         <v>110000</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="15">
         <v>56200</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="11">
         <v>14.1</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="1"/>
         <v>310000</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="14">
         <v>170022</v>
       </c>
       <c r="I23" s="10">
@@ -5757,17 +5705,17 @@
         <f t="shared" si="0"/>
         <v>115000</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="15">
         <v>56500</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="11">
         <v>13.9</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="1"/>
         <v>320000</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="14">
         <v>176903</v>
       </c>
       <c r="I24" s="10">
@@ -5779,17 +5727,17 @@
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="15">
         <v>56400</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="11">
         <v>14.2</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" si="1"/>
         <v>330000</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="14">
         <v>181078</v>
       </c>
       <c r="I25" s="10">
@@ -5801,17 +5749,17 @@
         <f t="shared" si="0"/>
         <v>125000</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="15">
         <v>56400</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="11">
         <v>14.3</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="1"/>
         <v>340000</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="14">
         <v>186162</v>
       </c>
       <c r="I26" s="10">
@@ -5823,17 +5771,17 @@
         <f t="shared" si="0"/>
         <v>130000</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="15">
         <v>56500</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="11">
         <v>14.3</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="1"/>
         <v>350000</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="14">
         <v>191326</v>
       </c>
       <c r="I27" s="10">
@@ -5845,17 +5793,17 @@
         <f t="shared" si="0"/>
         <v>135000</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="15">
         <v>56700</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="11">
         <v>14.1</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="1"/>
         <v>360000</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="14">
         <v>197552</v>
       </c>
       <c r="I28" s="10">
@@ -5867,17 +5815,17 @@
         <f t="shared" si="0"/>
         <v>140000</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="15">
         <v>57700</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="11">
         <v>14.1</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" si="1"/>
         <v>370000</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="14">
         <v>198104</v>
       </c>
       <c r="I29" s="10">
@@ -5889,17 +5837,17 @@
         <f t="shared" si="0"/>
         <v>145000</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="15">
         <v>58400</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="11">
         <v>14.1</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="1"/>
         <v>380000</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="14">
         <v>198198</v>
       </c>
       <c r="I30" s="10">
@@ -5911,17 +5859,17 @@
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="15">
         <v>56400</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="11">
         <v>14.3</v>
       </c>
       <c r="G31" s="2">
         <f t="shared" si="1"/>
         <v>390000</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="14">
         <v>198842</v>
       </c>
       <c r="I31" s="10">
@@ -5929,13 +5877,13 @@
       </c>
     </row>
     <row r="32" spans="2:9">
-      <c r="C32" s="13"/>
-      <c r="D32" s="16"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="11"/>
       <c r="G32" s="2">
         <f>G31+10000</f>
         <v>400000</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="14">
         <v>199756</v>
       </c>
       <c r="I32" s="10">
@@ -5943,46 +5891,49 @@
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="C33" s="13"/>
-      <c r="D33" s="16"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="11"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="C34" s="13"/>
-      <c r="D34" s="16"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="11"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="C35" s="13"/>
-      <c r="D35" s="16"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="11"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="C36" s="13"/>
-      <c r="D36" s="16"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="11"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="C37" s="13"/>
-      <c r="D37" s="16"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="11"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="H38" s="11"/>
-      <c r="I38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="H39" s="11"/>
-      <c r="I39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="H40" s="11"/>
-      <c r="I40" s="12"/>
+      <c r="D40" s="13"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1"/>
@@ -6018,13 +5969,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" t="s">
+      <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="17">
+      <c r="C1" s="9">
         <f t="array" ref="C1">MIN(IF(NOT(ISNA(Helpers!E2:E151)),Helpers!E2:E151))</f>
         <v>5000</v>
       </c>
@@ -6048,10 +5999,11 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="9">
         <f t="array" ref="C2">MAX(IF(NOT(ISNA(Helpers!E2:E151)),Helpers!E2:E151))</f>
         <v>150000</v>
       </c>
@@ -6081,10 +6033,11 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="9">
         <f t="array" ref="C3">MIN(IF(NOT(ISNA(Helpers!I2:I151)),Helpers!I2:I151))</f>
         <v>100000</v>
       </c>
@@ -6114,10 +6067,11 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="9">
         <f t="array" ref="C4">MAX(IF(NOT(ISNA(Helpers!I2:I151)),Helpers!I2:I151))</f>
         <v>400000</v>
       </c>
@@ -6147,7 +6101,8 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="2">
@@ -6180,7 +6135,8 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="2">
@@ -6213,6 +6169,8 @@
       </c>
     </row>
     <row r="7" spans="1:11">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="E7">
         <f>IF(OR(ISBLANK('Latency Data'!$B7), NOT(Toggles!$B$3)),NA(),'Latency Data'!$B7)</f>
         <v>30000</v>
@@ -6239,6 +6197,8 @@
       </c>
     </row>
     <row r="8" spans="1:11">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="E8">
         <f>IF(OR(ISBLANK('Latency Data'!$B8), NOT(Toggles!$B$3)),NA(),'Latency Data'!$B8)</f>
         <v>35000</v>
@@ -6265,10 +6225,10 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" t="s">
+      <c r="A9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2" t="e">
@@ -6301,7 +6261,8 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="B10" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="2" t="e">
@@ -6334,10 +6295,10 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" t="s">
+      <c r="A11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C11">
@@ -6370,7 +6331,8 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="B12" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C12">
@@ -6429,7 +6391,7 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="C14" s="17"/>
+      <c r="C14" s="9"/>
       <c r="E14">
         <f>IF(OR(ISBLANK('Latency Data'!$B14), NOT(Toggles!$B$3)),NA(),'Latency Data'!$B14)</f>
         <v>65000</v>

</xml_diff>

<commit_message>
Moved chart data labels data to the chart page for easy edits Changed teh chart line colors to be less confusing
</commit_message>
<xml_diff>
--- a/RequestedOps vs. Achieved at Latency.xlsx
+++ b/RequestedOps vs. Achieved at Latency.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Requested Ops</t>
   </si>
@@ -138,13 +138,43 @@
   <si>
     <t>Max Total</t>
   </si>
+  <si>
+    <t>Note 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To change the legend </t>
+  </si>
+  <si>
+    <t>Data set 1</t>
+  </si>
+  <si>
+    <t>Latency label</t>
+  </si>
+  <si>
+    <t>OPs label</t>
+  </si>
+  <si>
+    <t>Data set 2</t>
+  </si>
+  <si>
+    <t>Set 1 Latency</t>
+  </si>
+  <si>
+    <t>Set 1 OPs</t>
+  </si>
+  <si>
+    <t>Set 2 Latency</t>
+  </si>
+  <si>
+    <t>Set 2 OPs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="#.00\ &quot;ms&quot;"/>
+    <numFmt numFmtId="164" formatCode="#.00\ &quot;ms&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -230,7 +260,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -241,14 +271,14 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -256,6 +286,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,21 +333,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Requested NFS OPS vs. Achieved OPS and Latency (verilog, 5</a:t>
+              <a:t>Requested NFS OPS vs. Achieved OPS and Latency</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> node </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>S210 </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>vs Nitro 4 node)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -389,14 +409,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="4"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Latency Data'!$D$1</c:f>
+              <c:f>'Latency and Ops Graph'!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Latency (ms) 1</c:v>
+                  <c:v>Set 1 Latency</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1356,11 +1376,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Latency Data'!$I$1</c:f>
+              <c:f>'Latency and Ops Graph'!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Latency (ms) 2</c:v>
+                  <c:v>Set 2 Latency</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2300,8 +2320,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="253748624"/>
-        <c:axId val="330259696"/>
+        <c:axId val="200838632"/>
+        <c:axId val="200875784"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2363,11 +2383,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Latency Data'!$C$1</c:f>
+              <c:f>'Latency and Ops Graph'!$N$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Achieved Ops 1</c:v>
+                  <c:v>Set 1 OPs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3301,14 +3321,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Latency Data'!$H$1</c:f>
+              <c:f>'Latency and Ops Graph'!$N$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Achieved Ops 2</c:v>
+                  <c:v>Set 2 OPs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4248,11 +4268,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="339620552"/>
-        <c:axId val="339620160"/>
+        <c:axId val="200880648"/>
+        <c:axId val="200878216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="253748624"/>
+        <c:axId val="200838632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="410000"/>
@@ -4283,12 +4303,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="330259696"/>
+        <c:crossAx val="200875784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="330259696"/>
+        <c:axId val="200875784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -4320,13 +4340,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="253748624"/>
+        <c:crossAx val="200838632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339620160"/>
+        <c:axId val="200878216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350000"/>
@@ -4357,13 +4377,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339620552"/>
+        <c:crossAx val="200880648"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339620552"/>
+        <c:axId val="200880648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4373,7 +4393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339620160"/>
+        <c:crossAx val="200878216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4991,9 +5011,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -5027,6 +5049,14 @@
       </c>
       <c r="B4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -5036,18 +5066,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:14">
       <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5057,8 +5091,17 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -5066,16 +5109,37 @@
         <f t="array" ref="D3">MAX(MAX(IF(NOT(ISNA(Helpers!F2:F151)),Helpers!F2:F151)),MAX(IF(NOT(ISNA(Helpers!J2:J151)),Helpers!J2:J151)))</f>
         <v>199756</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="M3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -5202,19 +5266,21 @@
       <c r="B1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="18" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>